<commit_message>
removed get tuned ucb
</commit_message>
<xml_diff>
--- a/EQTime.xlsx
+++ b/EQTime.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7169C895-861D-46D9-9031-8019B72D7A0F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AEEE4F9D-FDE0-459B-805E-E5128E389111}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26083" windowHeight="10963" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>ProjeDate</t>
   </si>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -705,6 +705,61 @@
         <v>1.8368055555555554E-2</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43331</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.7905092592592594E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43336</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3.6331018518518519E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43338</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2.2349537037037032E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43343</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3.6724537037037035E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43346</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1.3530092592592594E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
make get_quality smarter. it will assign ambiguous quality given one input
</commit_message>
<xml_diff>
--- a/EQTime.xlsx
+++ b/EQTime.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AEEE4F9D-FDE0-459B-805E-E5128E389111}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C0FE2B-6E85-441C-B1C1-A6CA638BAC9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26083" windowHeight="10963" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t>ProjeDate</t>
   </si>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -760,6 +760,28 @@
         <v>1.3530092592592594E-2</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43351</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43359</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2.5925925925925925E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>